<commit_message>
[MOD]     excel_automation.py     add function which sweaps all the files in Downloads Directory and process excels
</commit_message>
<xml_diff>
--- a/sample_workbook.xlsx
+++ b/sample_workbook.xlsx
@@ -9,6 +9,15 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="국내" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="국외" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합4" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합5" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합6" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합7" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합8" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="종합9" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -634,7 +643,7 @@
     </row>
     <row r="10">
       <c r="B10" s="19" t="n">
-        <v>43793.90208333333</v>
+        <v>43793.90208333332</v>
       </c>
       <c r="C10" s="14" t="n">
         <v>8</v>
@@ -886,6 +895,1203 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1480,4 +2686,2398 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>20800</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티머니택시(법인)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>교통비</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>씨유호박점</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11.12</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11.15</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NICE-주차료결제</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11.19</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>롯데쇼핑인천공항점</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11.20</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>51000</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>케이에너지구룡주유소</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>주유비</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>호반베르디움아브뉴프랑판교지점</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>주차비</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.25</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>233900</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(주)이마트</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>연구소 간식 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>73000</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>한국정</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>자산관리</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11.28</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>200100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>쿠팡-정기배송</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>물품 구매</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>미래석유(주)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>카와이</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>다날_수기ARS</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.30</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>오래</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>7749</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Amazon Prime</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>배송비</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7208</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PAYPAL *JIN9000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11.26</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>635754</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>AMZN Mktp US*7R06Z8A23</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>** 직접입력하세요. **</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>